<commit_message>
Update "Satisfied By" for a few reqs.
</commit_message>
<xml_diff>
--- a/SGV Requirements.xlsx
+++ b/SGV Requirements.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="50">
   <si>
     <t/>
   </si>
@@ -165,6 +165,12 @@
   <si>
     <t>Monitor Vessel Location and Status
 Communicate With Vessel</t>
+  </si>
+  <si>
+    <t>Waste Transfer Subsystem</t>
+  </si>
+  <si>
+    <t>Navigation Subsystem</t>
   </si>
 </sst>
 </file>
@@ -222,7 +228,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -238,6 +244,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="true"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="true"/>
@@ -811,13 +820,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="43.85546875" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="74.85546875" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="15.7109375" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="13.7109375" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" width="14.140625" collapsed="false"/>
-    <col min="6" max="6" customWidth="true" width="13.0" collapsed="false"/>
-    <col min="7" max="7" customWidth="true" width="15.85546875" collapsed="false"/>
+    <col min="1" max="1" customWidth="true" width="43.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="74.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="15.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -844,324 +853,324 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="G2" s="6" t="s">
+      <c r="D2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="7" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="G3" s="6" t="s">
+      <c r="D3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="7" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D4" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="G4" s="6" t="s">
+      <c r="D4" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G4" s="7" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="G5" s="6" t="s">
+      <c r="D5" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G5" s="7" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="G6" s="6" t="s">
+      <c r="D6" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G6" s="7" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="G7" s="6" t="s">
+      <c r="D7" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G7" s="7" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D8" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="G8" s="6" t="s">
+      <c r="D8" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G8" s="7" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D9" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="G9" s="6" t="s">
+      <c r="D9" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G9" s="7" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="G10" s="6" t="s">
+      <c r="D10" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G10" s="7" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="G11" s="6" t="s">
+      <c r="D11" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G11" s="7" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D12" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="G12" s="6" t="s">
+      <c r="D12" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G12" s="7" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="G13" s="6" t="s">
+      <c r="C13" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G13" s="7" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="G14" s="6" t="s">
+      <c r="C14" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G14" s="7" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="G15" s="6" t="s">
+      <c r="C15" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G15" s="7" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>